<commit_message>
Normalized noise level values for the test set
</commit_message>
<xml_diff>
--- a/noise/test results/NOISE DIFF TEST RESULTS.xlsx
+++ b/noise/test results/NOISE DIFF TEST RESULTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\OneDrive\Skrivebord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\OneDrive\Skrivebord\computer-vision\noise\test results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6F0CD9-4F9E-4079-B2EB-353D359AFDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8B9FC5-E036-4CF0-9B7C-07A3D523538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E756F257-9AD7-429E-9DB3-859F52EF5B3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E756F257-9AD7-429E-9DB3-859F52EF5B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>original</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Using mean squared error - rgb image - color channels separated</t>
+  </si>
+  <si>
+    <t>Using mean squared error - rgb image - color channels separated - normalized (values between 0 and 5)</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -155,10 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7CCB7-5A28-472B-A2F9-2210C1271888}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,34 +775,34 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>3.6027</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>2.5482</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>0.28860000000000002</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>8.0199999999999994E-2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>0.84989999999999999</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
         <v>0.3382</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14">
         <v>0.19689999999999999</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14">
         <v>6.9010000000000002E-2</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14">
         <v>0.46929999999999999</v>
       </c>
     </row>
@@ -808,34 +810,34 @@
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>4.2486899999999999</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.36249999999999999</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>3.6884999999999999</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>1.0894999999999999</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>0.3624</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>1.3266</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
         <v>1.4045000000000001</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15">
         <v>1.1361000000000001</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15">
         <v>0.5423</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15">
         <v>0.88980000000000004</v>
       </c>
     </row>
@@ -843,34 +845,34 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>8.1216000000000008</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>2.4064000000000001</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>8.7040000000000006</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>8.9413</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>1.9882</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
         <v>4.8727</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
         <v>15.5327</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16">
         <v>10.5913</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16">
         <v>4.8619000000000003</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16">
         <v>3.5895000000000001</v>
       </c>
     </row>
@@ -878,34 +880,34 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>14.487299999999999</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>7.1081000000000003</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>20.0885</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
         <v>23.399799999999999</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>7.5750999999999999</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <v>12.292299999999999</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>36.322800000000001</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <v>29.376200000000001</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17">
         <v>16.0992</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17">
         <v>13.286</v>
       </c>
     </row>
@@ -913,34 +915,34 @@
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>22.970800000000001</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>16.974499999999999</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>38.054600000000001</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>43.675800000000002</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>17.6645</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18">
         <v>22.806699999999999</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18">
         <v>61.595599999999997</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
         <v>54.139600000000002</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18">
         <v>30.342300000000002</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18">
         <v>29.597100000000001</v>
       </c>
     </row>
@@ -948,48 +950,36 @@
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>35.772399999999998</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>32.276299999999999</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>64.355900000000005</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>75.338700000000003</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>33.306199999999997</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
         <v>38.0946</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19">
         <v>91.317300000000003</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
         <v>88.200100000000006</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19">
         <v>53.4803</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19">
         <v>54.8658</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1082,19 +1072,19 @@
       <c r="F26">
         <v>1.0657000000000001</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26">
         <v>2.7618999999999998</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26">
         <v>6.3634000000000004</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26">
         <v>4.4981999999999998</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26">
         <v>1.9708000000000001</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26">
         <v>1.9288000000000001</v>
       </c>
     </row>
@@ -1105,7 +1095,7 @@
       <c r="B27">
         <v>15.4092</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>5.8888999999999996</v>
       </c>
       <c r="D27">
@@ -1140,7 +1130,7 @@
       <c r="B28">
         <v>33.731000000000002</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>22.131900000000002</v>
       </c>
       <c r="D28">
@@ -1175,7 +1165,7 @@
       <c r="B29">
         <v>59.160600000000002</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>41.525799999999997</v>
       </c>
       <c r="D29">
@@ -1210,7 +1200,7 @@
       <c r="B30">
         <v>94.959699999999998</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>66.111400000000003</v>
       </c>
       <c r="D30">
@@ -1236,6 +1226,218 @@
       </c>
       <c r="K30">
         <v>120.8165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>0.16</v>
+      </c>
+      <c r="C36">
+        <v>0.02</v>
+      </c>
+      <c r="D36">
+        <v>0.13</v>
+      </c>
+      <c r="E36">
+        <v>0.09</v>
+      </c>
+      <c r="F36">
+        <v>0.02</v>
+      </c>
+      <c r="G36">
+        <v>0.06</v>
+      </c>
+      <c r="H36">
+        <v>0.15</v>
+      </c>
+      <c r="I36">
+        <v>0.11</v>
+      </c>
+      <c r="J36">
+        <v>0.05</v>
+      </c>
+      <c r="K36">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <v>0.36</v>
+      </c>
+      <c r="C37">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D37">
+        <v>0.45</v>
+      </c>
+      <c r="E37">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F37">
+        <v>0.19</v>
+      </c>
+      <c r="G37">
+        <v>0.33</v>
+      </c>
+      <c r="H37">
+        <v>0.88</v>
+      </c>
+      <c r="I37">
+        <v>0.69</v>
+      </c>
+      <c r="J37">
+        <v>0.37</v>
+      </c>
+      <c r="K37">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>0.8</v>
+      </c>
+      <c r="C38">
+        <v>0.52</v>
+      </c>
+      <c r="D38">
+        <v>1.19</v>
+      </c>
+      <c r="E38">
+        <v>1.46</v>
+      </c>
+      <c r="F38">
+        <v>0.64</v>
+      </c>
+      <c r="G38">
+        <v>0.75</v>
+      </c>
+      <c r="H38">
+        <v>2.09</v>
+      </c>
+      <c r="I38">
+        <v>1.75</v>
+      </c>
+      <c r="J38">
+        <v>0.97</v>
+      </c>
+      <c r="K38">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39">
+        <v>1.4</v>
+      </c>
+      <c r="C39">
+        <v>0.98</v>
+      </c>
+      <c r="D39">
+        <v>2.27</v>
+      </c>
+      <c r="E39">
+        <v>2.68</v>
+      </c>
+      <c r="F39">
+        <v>1.26</v>
+      </c>
+      <c r="G39">
+        <v>1.29</v>
+      </c>
+      <c r="H39">
+        <v>3.44</v>
+      </c>
+      <c r="I39">
+        <v>3.17</v>
+      </c>
+      <c r="J39">
+        <v>1.89</v>
+      </c>
+      <c r="K39">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C40">
+        <v>1.56</v>
+      </c>
+      <c r="D40">
+        <v>3.74</v>
+      </c>
+      <c r="E40">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="F40">
+        <v>2.1</v>
+      </c>
+      <c r="G40">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="H40">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>3.16</v>
+      </c>
+      <c r="K40">
+        <v>2.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>